<commit_message>
alyael xi rpl 1 eskul itc lat rumus excel
</commit_message>
<xml_diff>
--- a/Alya Elidhiya XI RPL 1 -ITC Lat Excel/Alya Elidhiya XI RPL 1 -LatExcel25rumus.xlsx
+++ b/Alya Elidhiya XI RPL 1 -ITC Lat Excel/Alya Elidhiya XI RPL 1 -LatExcel25rumus.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\Alya Elidhiya XI RPL 1 -ITC Lat Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7305" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -1228,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,12 +1294,18 @@
         <f>SUM(C2:E2)</f>
         <v>25000000</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3">
+        <f>AVERAGE(C2,D2,E2)</f>
+        <v>8333333.333333333</v>
+      </c>
       <c r="H2" s="2" t="str">
         <f>IF(F2&gt;30000000,"LULUS","TIDAK LULUS")</f>
         <v>TIDAK LULUS</v>
       </c>
-      <c r="I2" s="4"/>
+      <c r="I2" s="4">
+        <f>RANK(F2,$F$2:$F$6,0)</f>
+        <v>4</v>
+      </c>
       <c r="K2" s="7" t="s">
         <v>21</v>
       </c>
@@ -1325,15 +1331,15 @@
         <v>33000000</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G6" si="1">AVERAGE(C3,D3,E3)</f>
+        <f>AVERAGE(C3,D3,E3)</f>
         <v>11000000</v>
       </c>
       <c r="H3" s="6" t="str">
-        <f t="shared" ref="H3:H6" si="2">IF(F3&gt;30000000,"LULUS","TIDAK LULUS")</f>
+        <f t="shared" ref="H3:H6" si="1">IF(F3&gt;30000000,"LULUS","TIDAK LULUS")</f>
         <v>LULUS</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I6" si="3">RANK(F3,$F$2:$F$6,0)</f>
+        <f>RANK(F3,$F$2:$F$6,0)</f>
         <v>2</v>
       </c>
       <c r="K3" s="7" t="s">
@@ -1361,7 +1367,7 @@
         <v>23000000</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G3:G6" si="2">AVERAGE(C4,D4,E4)</f>
         <v>7666666.666666667</v>
       </c>
       <c r="H4" s="6" t="str">
@@ -1369,7 +1375,7 @@
         <v>TIDAK LULUS</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I3:I6" si="3">RANK(F4,$F$2:$F$6,0)</f>
         <v>5</v>
       </c>
       <c r="K4" s="7" t="s">
@@ -1397,11 +1403,11 @@
         <v>29000000</v>
       </c>
       <c r="G5" s="3">
+        <f t="shared" si="2"/>
+        <v>9666666.666666666</v>
+      </c>
+      <c r="H5" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>9666666.666666666</v>
-      </c>
-      <c r="H5" s="6" t="str">
-        <f t="shared" si="2"/>
         <v>TIDAK LULUS</v>
       </c>
       <c r="I5" s="4">
@@ -1433,11 +1439,11 @@
         <v>39250000</v>
       </c>
       <c r="G6" s="3">
+        <f t="shared" si="2"/>
+        <v>13083333.333333334</v>
+      </c>
+      <c r="H6" s="6" t="str">
         <f t="shared" si="1"/>
-        <v>13083333.333333334</v>
-      </c>
-      <c r="H6" s="6" t="str">
-        <f t="shared" si="2"/>
         <v>LULUS</v>
       </c>
       <c r="I6" s="4">
@@ -2220,7 +2226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>